<commit_message>
removed old test data
</commit_message>
<xml_diff>
--- a/templates/Final/Conjoint_Config_Template_Annotated_Final.xlsx
+++ b/templates/Final/Conjoint_Config_Template_Annotated_Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duncan/Documents/Turas/templates/Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2F141E-912C-6C4B-A013-6E6FD1F84A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38288B65-0699-2C45-80F7-C59EC4116AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27920" yWindow="2140" windowWidth="20120" windowHeight="23680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="290">
   <si>
     <t>Setting</t>
   </si>
@@ -307,12 +307,6 @@
     <t>Respondent identifier</t>
   </si>
   <si>
-    <t xml:space="preserve"> Choice task identifier ✓</t>
-  </si>
-  <si>
-    <t>Alternative within each choice set</t>
-  </si>
-  <si>
     <t>Attribute column</t>
   </si>
   <si>
@@ -3127,13 +3121,608 @@
   </si>
   <si>
     <t>Your sheet must consist of the white area only</t>
+  </si>
+  <si>
+    <t>none_label</t>
+  </si>
+  <si>
+    <t>alternative_id_column</t>
+  </si>
+  <si>
+    <t>rating_variable</t>
+  </si>
+  <si>
+    <t>Column with ratings (only for analysis_type='rating')</t>
+  </si>
+  <si>
+    <t>Label for "None of these" option</t>
+  </si>
+  <si>
+    <t>Column identifying alternatives within choice sets - in alchemer data this seems to be called the cardnumber</t>
+  </si>
+  <si>
+    <t>so must be a comma spearated list!</t>
+  </si>
+  <si>
+    <t>min_responses_per_level</t>
+  </si>
+  <si>
+    <t>minimum number of times a level should be selected. Issues warning if below threshold. - default is 10.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Choice task identifier  - may be called stnumber in alchemer</t>
+  </si>
+  <si>
+    <t>Alternative within each choice set - may be called cardnumber in alchemer</t>
+  </si>
+  <si>
+    <t>Hard Limits (Will Error)</t>
+  </si>
+  <si>
+    <t>Attributes:</t>
+  </si>
+  <si>
+    <r>
+      <t>Minimum:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 2 attributes (modules/conjoint/R/01_config.R:230)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Maximum:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> No hard limit, but </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>warning issued if &gt; 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (line 234)</t>
+    </r>
+  </si>
+  <si>
+    <t>Levels per Attribute:</t>
+  </si>
+  <si>
+    <r>
+      <t>Minimum:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 2 levels per attribute (line 262)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Maximum:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> No hard limit, but </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>warning issued if &gt; 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (line 270)</t>
+    </r>
+  </si>
+  <si>
+    <t>Products/Alternatives per Choice Set:</t>
+  </si>
+  <si>
+    <r>
+      <t>No hard limits</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> - the code accepts any number</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Validation only checks for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unbalanced sets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (warning if inconsistent)</t>
+    </r>
+  </si>
+  <si>
+    <t>Best Practice Recommendations (USER_MANUAL.md:936-952)</t>
+  </si>
+  <si>
+    <t>✅ Optimal Design:</t>
+  </si>
+  <si>
+    <r>
+      <t>Attributes:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 4-6 (optimal range)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Levels per attribute:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 3-4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Choice sets per respondent:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 8-12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Alternatives per choice set:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 3-4</t>
+    </r>
+  </si>
+  <si>
+    <t>❌ Not Recommended:</t>
+  </si>
+  <si>
+    <r>
+      <t>Attributes:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> &gt;8 (respondent burden, line 947)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Levels per attribute:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> &gt;6 (too many parameters, line 948)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Choice sets:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> &lt;6 (insufficient data, line 949)</t>
+    </r>
+  </si>
+  <si>
+    <t>Sample Size Requirements</t>
+  </si>
+  <si>
+    <r>
+      <t>Formula</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (modules/conjoint/R/02_data.R:324):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">recommended_n </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4078F2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF383A42"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> max(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB76B01"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>300</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF383A42"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB76B01"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>300</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF383A42"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> × (n_attributes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4078F2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB76B01"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF383A42"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) × (max_levels</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4078F2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB76B01"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF383A42"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>Examples:</t>
+  </si>
+  <si>
+    <r>
+      <t>4 attributes, 4 levels max:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 300 respondents minimum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6 attributes, 4 levels max:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 450 respondents minimum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6 attributes, 6 levels max:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 675 respondents minimum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Warning issued if below recommended sample size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (line 326)</t>
+    </r>
+  </si>
+  <si>
+    <t>Summary Table</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Minimum (Error)</t>
+  </si>
+  <si>
+    <t>Warning Threshold</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>&gt;6</t>
+  </si>
+  <si>
+    <t>Levels/Attribute</t>
+  </si>
+  <si>
+    <t>Alternatives/Set</t>
+  </si>
+  <si>
+    <t>(no limit)</t>
+  </si>
+  <si>
+    <t>(unbalanced)</t>
+  </si>
+  <si>
+    <t>Choice Sets/Resp</t>
+  </si>
+  <si>
+    <t>(none)</t>
+  </si>
+  <si>
+    <t>Sample Size</t>
+  </si>
+  <si>
+    <t>&lt;300 (adjusted)</t>
+  </si>
+  <si>
+    <t>300+</t>
+  </si>
+  <si>
+    <r>
+      <t>The code is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>flexible</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> but issues </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>warnings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> to guide you toward designs that produce reliable results.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3226,6 +3815,35 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -3274,7 +3892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3293,6 +3911,12 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3598,7 +4222,7 @@
   <dimension ref="C3:F221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3608,7 +4232,7 @@
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.2">
@@ -3624,7 +4248,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.2">
@@ -3632,7 +4256,7 @@
         <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.2">
@@ -3640,7 +4264,7 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.2">
@@ -3648,7 +4272,7 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.2">
@@ -3656,7 +4280,7 @@
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.2">
@@ -3664,7 +4288,7 @@
         <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.2">
@@ -3672,90 +4296,90 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C18" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C19" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C20" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C22" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C23" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C24" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C25" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C26" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C27" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C29" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="3:3" ht="23" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="3:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C34" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="3:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C38" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="3:6" ht="18" x14ac:dyDescent="0.2">
@@ -3763,10 +4387,10 @@
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>34</v>
@@ -3777,630 +4401,630 @@
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="F41" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="44" spans="3:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C44" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="3:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C46" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="3:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C47" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="3:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C48" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C49" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C50" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C51" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C55" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C57" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C59" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C61" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C63" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C65" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C66" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C67" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C68" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C70" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C72" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C73" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C74" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C75" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C76" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C80" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C82" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C84" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="86" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C86" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C88" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C89" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="91" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C91" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C93" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C95" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C96" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="101" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C101" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="103" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C103" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="104" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C104" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="105" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C105" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C106" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="107" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C107" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="111" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C111" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C113" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="115" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C115" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="117" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C117" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="119" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C119" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="121" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C121" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="122" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C122" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="123" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C123" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="124" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C124" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="126" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C126" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C128" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C129" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C130" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C131" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C132" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C133" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C134" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C135" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C136" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C137" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C139" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C140" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C141" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C142" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="144" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C144" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="146" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C146" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="147" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C147" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="148" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C148" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="149" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C149" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="150" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C150" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="151" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C151" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="155" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C155" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="157" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C157" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="159" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C159" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="161" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C161" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="163" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C163" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C165" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C166" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C167" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C168" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C169" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="171" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C171" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C173" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C174" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C175" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C176" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C177" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C179" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C180" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C181" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C182" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C183" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C184" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C185" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C186" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C187" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C188" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C189" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C190" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C191" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="193" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C193" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="195" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C195" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="196" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C196" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="197" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C197" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="198" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C198" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="199" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C199" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="200" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C200" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="204" spans="3:3" ht="23" x14ac:dyDescent="0.25">
       <c r="C204" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="206" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C206" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="208" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C208" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="209" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C209" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="210" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C210" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="212" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C212" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="214" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C214" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="215" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C215" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="216" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C216" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="217" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C217" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="221" spans="3:3" ht="18" x14ac:dyDescent="0.2">
       <c r="C221" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -4411,10 +5035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4428,7 +5052,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -4462,7 +5086,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4530,322 +5154,376 @@
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="8"/>
+    <row r="9" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="D10" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>29</v>
+        <v>240</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>30</v>
+        <v>238</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8" t="s">
+      <c r="F19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8" t="s">
+      <c r="F20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="8" t="s">
+      <c r="D21" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="D19" s="5"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="D25" s="5"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>86</v>
+        <v>107</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>91</v>
+      <c r="A38" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>93</v>
+      <c r="A42" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>97</v>
+      <c r="A46" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>99</v>
+      <c r="A50" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A58" s="9" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -4855,10 +5533,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B15" sqref="B15:E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4870,7 +5548,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -4900,7 +5578,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -4914,6 +5592,9 @@
       </c>
       <c r="C6" s="8" t="s">
         <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4964,35 +5645,485 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="2:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="2:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="2:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="2:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+    <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="B15" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="2:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="B22" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="2:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="B34" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="2:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="2:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="B43" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="2:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="B51" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B63" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="2:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="B67" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="E69" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B70" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C70" s="6">
+        <v>2</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="E70" s="20">
+        <v>45753</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B71" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="C71" s="6">
+        <v>2</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="E71" s="20">
+        <v>45720</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B72" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C72" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="E72" s="20">
+        <v>45720</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B73" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="E73" s="20">
+        <v>45881</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B74" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B76" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>